<commit_message>
Cleaning up old unused files before making repo public
</commit_message>
<xml_diff>
--- a/plots/Tables_T1-T6.xlsx
+++ b/plots/Tables_T1-T6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elwel\OneDrive\Desktop\aquatic_data\git\BOSCH\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2983392F-8687-43B0-98EE-1D88DD142B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DFE481-3656-49D0-A7CA-1FFF8A5C0269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F8FC7950-181F-4A0A-89C3-A717DF6795FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{F8FC7950-181F-4A0A-89C3-A717DF6795FB}"/>
   </bookViews>
   <sheets>
     <sheet name="T1_bodyLengthYr" sheetId="2" r:id="rId1"/>
@@ -116,9 +116,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,27 +260,6 @@
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -288,8 +267,41 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -671,7 +683,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,41 +695,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -725,58 +707,73 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1156,702 +1153,704 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E2CEDA-AAF0-4B9C-9287-4ADC12013DA8}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="9">
         <v>-0.20399999999999999</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="8">
         <v>5.569</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="8">
         <v>-0.53700000000000003</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="8">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="9">
         <v>0.17499999999999999</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="8">
         <v>2.5760000000000001</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="8">
         <v>2.5579999999999998</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="8">
         <v>0.38200000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="9">
         <v>-1.1639999999999999</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="8">
         <v>2.1619999999999999</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="8">
         <v>-0.21</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="8">
         <v>0.11899999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="12">
         <v>0.24399999999999999</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="13">
         <v>3.1E-2</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="13">
         <v>0.83399999999999996</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="13">
         <v>0.90500000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="9">
         <v>-8.3000000000000004E-2</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="8">
         <v>-6.1059999999999999</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="8">
         <v>-7.0730000000000004</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="8">
         <v>-0.41399999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="9">
         <v>0.08</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="8">
         <v>1.266</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="8">
         <v>1.3009999999999999</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="8">
         <v>0.214</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="9">
         <v>-1.04</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="8">
         <v>-4.8220000000000001</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="8">
         <v>-5.4379999999999997</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="8">
         <v>-1.94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="12">
         <v>0.29899999999999999</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="13">
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="8">
         <v>-20.23</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="8">
         <v>-4.0780000000000003</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="8">
         <v>-0.52600000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="9">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="8">
         <v>1.8360000000000001</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="8">
         <v>1.6359999999999999</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="8">
         <v>0.182</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="9">
         <v>-4.8040000000000003</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="8">
         <v>-11.019</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="8">
         <v>-2.492</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="8">
         <v>-2.883</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="13">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="8">
         <v>5.2960000000000003</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="8">
         <v>-3.3940000000000001</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="8">
         <v>0.36199999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="9">
         <v>0.26500000000000001</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="8">
         <v>5.69</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="8">
         <v>5.7649999999999997</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="8">
         <v>0.59</v>
       </c>
-      <c r="I15" s="17"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="9">
         <v>-2.419</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="8">
         <v>0.93100000000000005</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="8">
         <v>-0.58899999999999997</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="8">
         <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="12">
         <v>1.6E-2</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="13">
         <v>0.35199999999999998</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="13">
         <v>0.55600000000000005</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="13">
         <v>0.53900000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="9">
         <v>-1.7549999999999999</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="8">
         <v>-20.125</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="8">
         <v>-16.024999999999999</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="8">
         <v>2.7120000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="9">
         <v>1.9650000000000001</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="8">
         <v>8.7249999999999996</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="8">
         <v>10.135</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="8">
         <v>3.8210000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="9">
         <v>-0.89300000000000002</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="8">
         <v>-2.306</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="8">
         <v>-1.581</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="8">
         <v>0.71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="12">
         <v>0.372</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="13">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="13">
         <v>0.114</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="13">
         <v>0.47799999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="8">
         <v>-24.603000000000002</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="8">
         <v>-9.5779999999999994</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="8">
         <v>1.127</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="9">
         <v>0.30099999999999999</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="8">
         <v>3.411</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="8">
         <v>3.3759999999999999</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="8">
         <v>0.51700000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="9">
         <v>-4.2409999999999997</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="8">
         <v>-7.2140000000000004</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="8">
         <v>-2.8370000000000002</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="8">
         <v>2.181</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="13">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="9">
         <v>-4.2000000000000003E-2</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="8">
         <v>52.097999999999999</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="8">
         <v>3.4239999999999999</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="8">
         <v>0.45900000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="9">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="8">
         <v>2.2559999999999998</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="8">
         <v>2.0830000000000002</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="8">
         <v>0.23100000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="9">
         <v>-0.432</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="8">
         <v>23.088000000000001</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="8">
         <v>1.6439999999999999</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="8">
         <v>1.9930000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="31">
+      <c r="C29" s="12">
         <v>0.66600000000000004</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="13">
         <v>0.1</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F29" s="13">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="9">
         <v>-0.34499999999999997</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="8">
         <v>-3.6509999999999998</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="8">
         <v>-7.8070000000000004</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="8">
         <v>0.24199999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="9">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="8">
         <v>2.5659999999999998</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="8">
         <v>2.5350000000000001</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="8">
         <v>0.86499999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="17" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="9">
         <v>-1.1910000000000001</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="8">
         <v>-1.423</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="8">
         <v>-3.08</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="8">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="31">
+      <c r="C33" s="12">
         <v>0.23400000000000001</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="13">
         <v>0.155</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="13">
         <v>2E-3</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="13">
         <v>0.78</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="8">
         <v>-17.826000000000001</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="8">
         <v>8.6549999999999994</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="8">
         <v>0.628</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="9">
         <v>0.126</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="8">
         <v>2.4670000000000001</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="8">
         <v>2.4140000000000001</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="8">
         <v>0.20899999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="21"/>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="9">
         <v>7.8630000000000004</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="8">
         <v>-7.2270000000000003</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="8">
         <v>3.585</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="8">
         <v>3.0070000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
-      <c r="B37" s="24" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="13">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
@@ -1868,6 +1867,7 @@
     <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1876,550 +1876,554 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+      <selection activeCell="C11" sqref="A1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="16">
         <v>-1.8249891867047299E-2</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="16">
         <v>1.04133621707859</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="16">
         <v>-5.3760891338450599E-2</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="16">
         <v>-2.1556520691698201E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="16">
         <v>2.72464075907572E-2</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="16">
         <v>0.40062684693735401</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="16">
         <v>0.39784835117935202</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="16">
         <v>5.9441261030599497E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="16">
         <v>-0.66980910442073005</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="16">
         <v>2.5992671860091998</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="16">
         <v>-0.135129104290833</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="16">
         <v>-0.36265247940485601</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="17">
         <v>0.50297948899372402</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="17">
         <v>9.3423026026047094E-3</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="17">
         <v>0.89250979931830898</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="17">
         <v>0.71686450228000997</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="18">
         <v>-5.7245211461448502E-2</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="16">
         <v>-3.0256901110739798</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="16">
         <v>-0.60300479997760204</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="16">
         <v>-3.8023410514548599E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="16">
         <v>8.7017313614674192E-3</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="16">
         <v>0.23796183672412999</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="16">
         <v>0.21059416149250301</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="16">
         <v>2.3027602482386E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="16">
         <v>-6.5786001754707</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="16">
         <v>-12.715022512545501</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="16">
         <v>-2.8633500364114699</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="16">
         <v>-1.6512101311299401</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
         <v>4.1918719119788898E-3</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="17">
         <v>9.8695675127376897E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="18">
         <v>-9.8598658931800795E-2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="16">
         <v>-7.9857791188551699E-2</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="16">
         <v>0.32970550546694599</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="16">
         <v>7.1595388184778702E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="16">
         <v>2.1945388931917002E-2</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="16">
         <v>0.46981795247471902</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="16">
         <v>0.47618028760110698</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="16">
         <v>4.8959408519928103E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="16">
         <v>-4.4929100704340099</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="16">
         <v>-0.16997603171166401</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="16">
         <v>0.69239637601953496</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="16">
         <v>1.4623417714623099</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="17">
         <v>0.86502898626176805</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="17">
         <v>0.48868844104341502</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="17">
         <v>0.14364757722883201</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="16">
         <v>-3.0482693048679101E-2</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="16">
         <v>-0.30754453589640801</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="16">
         <v>-0.829368659641471</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="16">
         <v>0.70638064495817898</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="16">
         <v>7.7821754527965997E-2</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="16">
         <v>0.628386814207331</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="16">
         <v>0.69388102203350099</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="16">
         <v>0.184539635247399</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="16">
         <v>-0.39169886664178</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="16">
         <v>-0.48941914270488801</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="16">
         <v>-1.19526061861572</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="16">
         <v>3.8277990742269701</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="17">
         <v>0.69528072754657899</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="17">
         <v>0.62454498630377298</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="17">
         <v>0.23198522111521</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="16">
         <v>1.6312846411688502E-2</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="16">
         <v>4.6859378258759996</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="16">
         <v>9.1050630883956502E-3</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="16">
         <v>8.16041704071295E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="16">
         <v>9.5218985096283595E-3</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="16">
         <v>0.21967421543113599</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="16">
         <v>0.20190388152676</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="16">
         <v>2.2237132659694601E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="16">
         <v>1.71319263644674</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="16">
         <v>21.331305618546502</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="16">
         <v>4.5096027969075497E-2</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="16">
         <v>3.6697253938246899</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="17">
         <v>8.6677105873967902E-2</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="17">
         <v>0.96403076742500105</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="16">
         <v>3.4444269116800999E-2</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="16">
         <v>0.88338235576519497</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="16">
         <v>-0.65794366905470503</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="16">
         <v>8.9833901223784596E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="16">
         <v>2.47044484335231E-2</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="16">
         <v>0.21624831468608</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="16">
         <v>0.21520040596042</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="16">
         <v>7.4263001574293205E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="16">
         <v>1.3942537195067</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="16">
         <v>4.0850369495252297</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="16">
         <v>-3.05735328945297</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="16">
         <v>1.2096723714286499</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="17">
         <v>0.163241001115529</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="17">
         <v>2.2330092121047901E-3</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="17">
         <v>0.22640463554495199</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="18">
         <v>3.7031427408544398E-2</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="16">
         <v>-6.7995787927245296E-2</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="16">
         <v>0.30973797774467599</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="16">
         <v>1.9014992067197201E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="16">
         <v>8.6114001151673999E-3</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="16">
         <v>0.162867762063303</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="16">
         <v>0.16031445932951799</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="16">
         <v>1.38228824804072E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="16">
         <v>4.3002795031344903</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="16">
         <v>-0.41749077328647</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="16">
         <v>1.93206513648295</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="16">
         <v>1.3756169955253199</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="17">
         <v>0.67631947172697204</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="17">
         <v>5.33514667670449E-2</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="17">
         <v>0.16894024208313299</v>
       </c>
     </row>
@@ -2442,275 +2446,278 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="16">
         <v>-4.0515784416660199E-2</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="16">
         <v>-4.5618845255242704</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="16">
         <v>-5.3773900140110298</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="16">
         <v>-0.23999272494990101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="16">
         <v>5.9664223887362498E-2</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="16">
         <v>0.94521488963356004</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="16">
         <v>0.96549482912235496</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="16">
         <v>0.15478753545384499</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="16">
         <v>-0.67906329416348599</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="16">
         <v>-4.8262935503405098</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="16">
         <v>-5.56956894207205</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="16">
         <v>-1.55046544443149</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="17">
         <v>0.49709775860267802</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="17">
         <v>0.12102984125404</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="18">
         <v>-8.6074691825343594E-2</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="16">
         <v>-3.7729778087981201</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="16">
         <v>-3.5905175847122899</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="16">
         <v>-0.21800427661584801</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="16">
         <v>4.1529019979656703E-2</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="16">
         <v>0.65362689485595304</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="16">
         <v>0.67329237755071603</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="16">
         <v>0.111920830536785</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="16">
         <v>-2.07263961122867</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="16">
         <v>-5.7723723403848197</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="16">
         <v>-5.3327762268359198</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="16">
         <v>-1.94784362812781</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="17">
         <v>3.8205831719535101E-2</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="17">
         <v>5.1433676665443101E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="16">
         <v>-0.10949635712325199</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="16">
         <v>-11.1549224888129</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="16">
         <v>-8.3147681876755595</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="16">
         <v>8.6678506039181202E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="16">
         <v>0.42505295413715599</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="16">
         <v>4.8160316821751197</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="16">
         <v>4.7599850479372101</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="16">
         <v>0.73311968210265799</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="16">
         <v>-0.25760639011561798</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="16">
         <v>-2.3162062097927998</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="16">
         <v>-1.7468055264750999</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="16">
         <v>0.118232408916616</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="17">
         <v>0.79671069752900303</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="17">
         <v>2.0547012301739699E-2</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="17">
         <v>8.0671077636795999E-2</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="17">
         <v>0.905883511441953</v>
       </c>
     </row>
@@ -2730,704 +2737,704 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500F118E-E1E2-4523-B1F4-E79E181278E8}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="16">
         <v>7.1929144657618196E-3</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="16">
         <v>5.6706986838982596</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="16">
         <v>-0.52436145229043396</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="16">
         <v>0.31652147373808798</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="16">
         <v>0.38537899256145403</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="16">
         <v>2.63665519068444</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="16">
         <v>2.6391997508312901</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="16">
         <v>0.52921611587637596</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="16">
         <v>1.8664521431107299E-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="16">
         <v>2.1507168263538601</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="16">
         <v>-0.19868198764616801</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="16">
         <v>0.598094926141718</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="17">
         <v>0.98510873111825803</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="17">
         <v>3.1498557433526302E-2</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="17">
         <v>0.84251151489877796</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="17">
         <v>0.54977659559238201</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="18">
         <v>0.25823978952568899</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="16">
         <v>-0.17871852042142</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="16">
         <v>-3.98746845295085</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="16">
         <v>-0.20048643905730401</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="16">
         <v>0.119007221441137</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="16">
         <v>1.19621469308738</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="16">
         <v>1.2366533110698901</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="16">
         <v>0.272199835287179</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="16">
         <v>2.1699505828175201</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="16">
         <v>-0.149403381729207</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="16">
         <v>-3.2244028437534298</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="16">
         <v>-0.73654136802024195</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="17">
         <v>3.0010589782334202E-2</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="17">
         <v>0.88123534344719301</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
         <v>1.26235683030695E-3</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="17">
         <v>0.46140130178428401</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="16">
         <v>-3.1637402153889001E-2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="16">
         <v>-10.542150466175</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="16">
         <v>-4.9464477111216896</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="16">
         <v>-0.849725449779001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="16">
         <v>0.20067563467723301</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="16">
         <v>1.7286187037377401</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="16">
         <v>1.69233354840247</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="16">
         <v>0.26228755421050698</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="16">
         <v>-0.157654426780683</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="16">
         <v>-6.09859794029766</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="16">
         <v>-2.9228562630522998</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="16">
         <v>-3.2396712544623001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="17">
         <v>0.87472911343960602</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="17">
         <v>3.4683658609275798E-3</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="17">
         <v>1.1966758119990001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="16">
         <v>1.37811457689137E-2</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="16">
         <v>9.6067715411073404</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="16">
         <v>11.191128262607601</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="16">
         <v>0.412033888981783</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="16">
         <v>0.38338565504276401</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="16">
         <v>5.5770160925415997</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="16">
         <v>5.9091207114718198</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="16">
         <v>0.74489278817791904</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="16">
         <v>3.594590874136E-2</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="16">
         <v>1.7225647876388499</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="16">
         <v>1.89387369272749</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="16">
         <v>0.55314522508622799</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="17">
         <v>0.97132548961991705</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="17">
         <v>8.4967257312030101E-2</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="17">
         <v>5.8241777124580001E-2</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="17">
         <v>0.58016397072493497</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="16">
         <v>-3.0080820013228999</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="16">
         <v>17.484575066667301</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="16">
         <v>-16.2174620699627</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="16">
         <v>20.199965617406701</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="16">
         <v>2.96369145249087</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="16">
         <v>10.375760524007999</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="16">
         <v>8.3679381743581107</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="16">
         <v>7.1040263172238802</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="16">
         <v>-1.0149781276302301</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="16">
         <v>1.68513672093824</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="16">
         <v>-1.93804754911525</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="16">
         <v>2.8434530948219399</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="17">
         <v>0.31011625380462199</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="17">
         <v>9.1962196335654695E-2</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="17">
         <v>5.26174216964541E-2</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="17">
         <v>4.4627577615370404E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="18">
         <v>-1.19485499960696</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="16">
         <v>-15.3525376354121</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="16">
         <v>-8.5860359351883897</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="16">
         <v>0.94216016096033905</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="16">
         <v>0.48021887824121401</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="16">
         <v>3.2433071780962401</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="16">
         <v>3.30589498767926</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="16">
         <v>0.72619148333182304</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="16">
         <v>-2.4881466634195499</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="16">
         <v>-4.7336057895150603</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="16">
         <v>-2.5971895559863998</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="16">
         <v>1.2973990780470701</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="17">
         <v>1.28410765478952E-2</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="17">
         <v>9.3990039207794106E-3</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="17">
         <v>0.19449390958521301</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="16">
         <v>-7.0878942180247796E-3</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="16">
         <v>27.286328755027402</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="16">
         <v>0.83250000113961897</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="16">
         <v>-8.9833050691101896E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="16">
         <v>0.35448521045159298</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="16">
         <v>2.5004491935520301</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="16">
         <v>2.4791712225896201</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="16">
         <v>0.343969092937632</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="16">
         <v>-1.9994894029556901E-2</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="16">
         <v>10.912570759442501</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="16">
         <v>0.335797702697609</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="16">
         <v>-0.26116605397273401</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="17">
         <v>0.98404744572667502</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="17">
         <v>0.73702342267015997</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="17">
         <v>0.79396445488249401</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="16">
         <v>-0.92168094412951296</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="16">
         <v>2.2243433675137401</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="16">
         <v>-6.4740812539743704</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="16">
         <v>3.0335726292148699</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="17" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="32">
+      <c r="C31" s="16">
         <v>0.51191778156491896</v>
       </c>
-      <c r="D31" s="32">
+      <c r="D31" s="16">
         <v>2.7994769149752701</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="16">
         <v>2.73588599394914</v>
       </c>
-      <c r="F31" s="32">
+      <c r="F31" s="16">
         <v>1.6714791563593101</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="17" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="32">
+      <c r="C32" s="16">
         <v>-1.80044721500386</v>
       </c>
-      <c r="D32" s="32">
+      <c r="D32" s="16">
         <v>0.79455678152409304</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="16">
         <v>-2.3663563716810101</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="16">
         <v>1.8149030561783199</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="24" t="s">
+      <c r="A33" s="10"/>
+      <c r="B33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="33">
+      <c r="C33" s="17">
         <v>7.1790051252116793E-2</v>
       </c>
-      <c r="D33" s="33">
+      <c r="D33" s="17">
         <v>0.42687136687543598</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="17">
         <v>1.7964143085574098E-2</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="17">
         <v>6.9538808809340893E-2</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="16">
         <v>-0.41264340828583601</v>
       </c>
-      <c r="D34" s="32">
+      <c r="D34" s="16">
         <v>-5.8112705296590699</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="16">
         <v>-0.337963759191239</v>
       </c>
-      <c r="F34" s="32">
+      <c r="F34" s="16">
         <v>-0.163600727076365</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="32">
+      <c r="C35" s="16">
         <v>0.40243067923825898</v>
       </c>
-      <c r="D35" s="32">
+      <c r="D35" s="16">
         <v>2.1055994902063899</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="16">
         <v>2.0635276350842</v>
       </c>
-      <c r="F35" s="32">
+      <c r="F35" s="16">
         <v>0.38812733194287802</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="17" t="s">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="32">
+      <c r="C36" s="16">
         <v>-1.0253776105412999</v>
       </c>
-      <c r="D36" s="32">
+      <c r="D36" s="16">
         <v>-2.75991258389289</v>
       </c>
-      <c r="E36" s="32">
+      <c r="E36" s="16">
         <v>-0.163779613824967</v>
       </c>
-      <c r="F36" s="32">
+      <c r="F36" s="16">
         <v>-0.42151302835957699</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="24" t="s">
+      <c r="A37" s="10"/>
+      <c r="B37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C37" s="17">
         <v>0.30518504834370802</v>
       </c>
-      <c r="D37" s="33">
+      <c r="D37" s="17">
         <v>5.7816829842543003E-3</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="17">
         <v>0.869904640767864</v>
       </c>
-      <c r="F37" s="33">
+      <c r="F37" s="17">
         <v>0.67338049967421498</v>
       </c>
     </row>
@@ -3455,551 +3462,554 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B18" sqref="A1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="16">
         <v>2.9202469654507599E-2</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="16">
         <v>1.12115591423389</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="16">
         <v>-1.56409868855075E-2</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="16">
         <v>-2.5614176544872601E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="16">
         <v>5.92458343104596E-2</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="16">
         <v>0.40534341408397701</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="16">
         <v>0.40573459936330902</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="16">
         <v>8.1358483261479098E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="16">
         <v>0.49290334070545799</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="16">
         <v>2.7659408671226502</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="16">
         <v>-3.8549798094744202E-2</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="16">
         <v>-0.31483104795047501</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="17">
         <v>0.62208088669707395</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="17">
         <v>5.6758825957934399E-3</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="17">
         <v>0.96924932782872197</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="17">
         <v>0.75288993672857996</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="16">
         <v>2.9627794325898401E-2</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="16">
         <v>-1.5666784214774101</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="16">
         <v>-0.37685259966831602</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="16">
         <v>-5.8499878016968002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="16">
         <v>2.4404009499058899E-2</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="16">
         <v>0.216293887056555</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="16">
         <v>0.21317120154614</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="16">
         <v>3.2032079527236003E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="16">
         <v>1.2140543678710201</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="16">
         <v>-7.2432857109261004</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="16">
         <v>-1.7678401066137801</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="16">
         <v>-1.82629035892681</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="17">
         <v>0.22472696367900899</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
         <v>7.70876379023957E-2</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="17">
         <v>6.7806536695108402E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="18">
         <v>6.60303164383787E-2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="16">
         <v>9.2030375859153704E-2</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="16">
         <v>1.5642644781980299</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="16">
         <v>0.11325622041366699</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="16">
         <v>3.2048893828671501E-2</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="16">
         <v>0.44754853171076198</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="16">
         <v>0.47464347426124198</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="16">
         <v>6.0422298997034801E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="16">
         <v>2.0602993910294298</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="16">
         <v>0.20563217023049099</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="16">
         <v>3.2956620348204102</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="16">
         <v>1.87441097564369</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="17">
         <v>3.93699281156061E-2</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="17">
         <v>0.83707824629870897</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="17">
         <v>9.8190060797920297E-4</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="17">
         <v>6.0873801873577001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="16">
         <v>-0.15156552265357501</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="16">
         <v>1.6376902988019799</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="16">
         <v>-1.0742744066110499</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="16">
         <v>1.21637024487111</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="16">
         <v>0.178209214244716</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="16">
         <v>0.81619610682041299</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="16">
         <v>0.75612468866462501</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="16">
         <v>0.450762102123897</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="16">
         <v>-0.850492065160253</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="16">
         <v>2.00649119141451</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="16">
         <v>-1.42076356283023</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="16">
         <v>2.6984749586086001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="17">
         <v>0.39505157010512598</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="17">
         <v>4.4803867628595798E-2</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="17">
         <v>0.15538550682545901</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="17">
         <v>6.9657978360457796E-3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="16">
         <v>5.61189306909608E-2</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="16">
         <v>2.4587528655258302</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="16">
         <v>-8.8111186726966995E-2</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="16">
         <v>4.19045405630043E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="16">
         <v>3.8276837273164402E-2</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="16">
         <v>0.261637773729756</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="16">
         <v>0.25864478530188501</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="16">
         <v>3.6287596213719901E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="16">
         <v>1.4661329067097499</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="16">
         <v>9.3975454326616497</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="16">
         <v>-0.340664848990191</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="16">
         <v>1.15478965088243</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
-      <c r="B21" s="24" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="17">
         <v>0.14261208245826701</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="17">
         <v>0.733355903846031</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="17">
         <v>0.248176576145651</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="16">
         <v>-5.9466067771333397E-2</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="16">
         <v>1.4354447959644201</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="16">
         <v>0.43040726419605002</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="16">
         <v>3.6388766791703601E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="16">
         <v>4.53125243086532E-2</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="16">
         <v>0.25759330766465799</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="16">
         <v>0.25472852748712699</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="16">
         <v>0.15275335429215101</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="16">
         <v>-1.31235389505716</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="16">
         <v>5.5725236380485503</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="16">
         <v>1.68967044422538</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="16">
         <v>0.238219101376377</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="17">
         <v>0.18940075536214199</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="17">
         <v>9.1091020701740799E-2</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="17">
         <v>0.81171116275671995</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="32">
+      <c r="C26" s="16">
         <v>-1.7412785815609299E-2</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="16">
         <v>0.109775160416881</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="16">
         <v>0.140067879862601</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="16">
         <v>-1.61427817145221E-2</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="16">
         <v>2.3968513004262702E-2</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="16">
         <v>0.16492869799245199</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="16">
         <v>0.16112858155981799</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="16">
         <v>2.84198533084793E-2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="16">
         <v>-0.72648586136789095</v>
       </c>
-      <c r="D28" s="32">
+      <c r="D28" s="16">
         <v>0.665591626885361</v>
       </c>
-      <c r="E28" s="32">
+      <c r="E28" s="16">
         <v>0.869292576814512</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="16">
         <v>-0.56801073317664796</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
-      <c r="B29" s="24" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="17">
         <v>0.46754097190576199</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="17">
         <v>0.50567215977456004</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="17">
         <v>0.384687122058675</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="17">
         <v>0.570027679908508</v>
       </c>
     </row>
@@ -4024,278 +4034,279 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF67989-6C5A-4053-9F85-8CF60C044418}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="23">
         <v>0.14899999999999999</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="23">
         <v>-0.308</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="23">
         <v>-2.6240000000000001</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="23">
         <v>-7.2999999999999995E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="26">
         <v>9.4E-2</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="26">
         <v>0.92600000000000005</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="26">
         <v>0.96</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="26">
         <v>0.216</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="26">
         <v>1.59</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="26">
         <v>-0.33300000000000002</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="26">
         <v>-2.7349999999999999</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="26">
         <v>-0.33800000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="30">
         <v>0.112</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="30">
         <v>0.73899999999999999</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="30">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="30">
         <v>0.73499999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="31">
         <v>0.16400000000000001</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="23">
         <v>-0.65200000000000002</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="23">
         <v>-2.1720000000000002</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="23">
         <v>-0.183</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="26">
         <v>6.2E-2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="26">
         <v>0.64800000000000002</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="26">
         <v>0.66500000000000004</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="26">
         <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="26">
         <v>2.661</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="26">
         <v>-1.0069999999999999</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="26">
         <v>-3.266</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="26">
         <v>-1.3220000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="15" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="30">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="30">
         <v>0.314</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="30">
         <v>1E-3</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="30">
         <v>0.186</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="23">
         <v>0.54600000000000004</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="23">
         <v>-7.03</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="23">
         <v>-10.176</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="23">
         <v>-0.05</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="26">
         <v>0.86</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="26">
         <v>5.8109999999999999</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="26">
         <v>5.923</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="26">
         <v>1.3009999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="26">
         <v>0.63500000000000001</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="26">
         <v>-1.21</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="26">
         <v>-1.718</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="26">
         <v>-3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="30">
         <v>0.52500000000000002</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="30">
         <v>0.22600000000000001</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="30">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="30">
         <v>0.97</v>
       </c>
     </row>

</xml_diff>